<commit_message>
Ch 20,21,22 and 24 complete
</commit_message>
<xml_diff>
--- a/API Learning/API Learn.xlsx
+++ b/API Learning/API Learn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dotnet\API Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC14483-AAFD-4652-9871-76577C9A4779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77D60B8-2473-44CF-AF95-414277E34605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -962,7 +962,7 @@
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
+      <selection pane="bottomLeft" activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -1548,7 +1548,9 @@
       <c r="C35" s="16"/>
       <c r="D35" s="27"/>
       <c r="E35" s="38"/>
-      <c r="F35" s="22"/>
+      <c r="F35" s="22">
+        <v>12</v>
+      </c>
       <c r="G35" s="30"/>
     </row>
     <row r="36" spans="1:7">
@@ -1561,7 +1563,9 @@
       <c r="C36" s="9"/>
       <c r="D36" s="18"/>
       <c r="E36" s="35"/>
-      <c r="F36" s="22"/>
+      <c r="F36" s="22">
+        <v>1.5</v>
+      </c>
       <c r="G36" s="31"/>
     </row>
     <row r="37" spans="1:7">
@@ -1617,7 +1621,9 @@
       <c r="C40" s="16"/>
       <c r="D40" s="21"/>
       <c r="E40" s="36"/>
-      <c r="F40" s="22"/>
+      <c r="F40" s="22">
+        <v>3</v>
+      </c>
       <c r="G40" s="30"/>
     </row>
     <row r="41" spans="1:7">

</xml_diff>

<commit_message>
Complate till 27 ch but documentation remaining ch 26 and 27 and chnage in folder structure in phase wise
</commit_message>
<xml_diff>
--- a/API Learning/API Learn.xlsx
+++ b/API Learning/API Learn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dotnet\API Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048CE5A9-7420-4022-8663-70D1013A03C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB1A2B1-43E2-4C8E-9232-0F0DA24A8FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -386,7 +386,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -601,13 +601,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -645,26 +669,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -682,6 +691,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -963,9 +993,9 @@
   <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
+      <selection pane="bottomLeft" activeCell="F54" sqref="F54:F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -997,7 +1027,7 @@
       <c r="F1" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="23" t="s">
         <v>79</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -1017,15 +1047,17 @@
       <c r="C2" s="9">
         <v>1</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="35"/>
-      <c r="F2" s="32">
+      <c r="E2" s="30"/>
+      <c r="F2" s="34">
         <v>4</v>
       </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="25"/>
+      <c r="G2" s="37">
+        <v>1</v>
+      </c>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="10"/>
@@ -1036,11 +1068,11 @@
       <c r="D3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="36"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25" t="s">
+      <c r="E3" s="31"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1053,9 +1085,9 @@
       <c r="D4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="36"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="30"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="36"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="10"/>
@@ -1066,9 +1098,9 @@
       <c r="D5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="36"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="30"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="36"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="10">
@@ -1083,11 +1115,11 @@
       <c r="D6" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="36"/>
-      <c r="F6" s="32">
+      <c r="E6" s="31"/>
+      <c r="F6" s="34">
         <v>3.5</v>
       </c>
-      <c r="G6" s="30"/>
+      <c r="G6" s="36"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="10"/>
@@ -1098,9 +1130,9 @@
       <c r="D7" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="36"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="30"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="36"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="10">
@@ -1115,11 +1147,11 @@
       <c r="D8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="36"/>
-      <c r="F8" s="32">
+      <c r="E8" s="31"/>
+      <c r="F8" s="34">
         <v>3.25</v>
       </c>
-      <c r="G8" s="30"/>
+      <c r="G8" s="36"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="10"/>
@@ -1130,9 +1162,9 @@
       <c r="D9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="30"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="36"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="10"/>
@@ -1143,9 +1175,9 @@
       <c r="D10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="30"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="36"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="10">
@@ -1160,11 +1192,11 @@
       <c r="D11" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="32">
-        <v>2</v>
-      </c>
-      <c r="G11" s="30"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="34">
+        <v>2</v>
+      </c>
+      <c r="G11" s="36"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="10"/>
@@ -1175,9 +1207,9 @@
       <c r="D12" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="36"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="30"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="36"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="10">
@@ -1192,11 +1224,11 @@
       <c r="D13" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="36"/>
-      <c r="F13" s="32">
+      <c r="E13" s="31"/>
+      <c r="F13" s="34">
         <v>4</v>
       </c>
-      <c r="G13" s="30"/>
+      <c r="G13" s="36"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="10"/>
@@ -1207,9 +1239,9 @@
       <c r="D14" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="36"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="30"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="36"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="10"/>
@@ -1220,9 +1252,9 @@
       <c r="D15" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="36"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="30"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="36"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="10">
@@ -1237,11 +1269,11 @@
       <c r="D16" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="36"/>
-      <c r="F16" s="32">
+      <c r="E16" s="31"/>
+      <c r="F16" s="34">
         <v>3</v>
       </c>
-      <c r="G16" s="30"/>
+      <c r="G16" s="36"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="10"/>
@@ -1252,9 +1284,9 @@
       <c r="D17" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="36"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="30"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="36"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="10"/>
@@ -1265,9 +1297,9 @@
       <c r="D18" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="36"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="30"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="36"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="14">
@@ -1282,11 +1314,11 @@
       <c r="D19" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="36"/>
+      <c r="E19" s="31"/>
       <c r="F19" s="22">
         <v>3</v>
       </c>
-      <c r="G19" s="30"/>
+      <c r="G19" s="36"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="7">
@@ -1301,11 +1333,13 @@
       <c r="D20" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="E20" s="35"/>
+      <c r="E20" s="30"/>
       <c r="F20" s="22">
         <v>4</v>
       </c>
-      <c r="G20" s="31"/>
+      <c r="G20" s="35">
+        <v>2</v>
+      </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="10">
@@ -1320,11 +1354,11 @@
       <c r="D21" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="36"/>
-      <c r="F21" s="32">
+      <c r="E21" s="31"/>
+      <c r="F21" s="34">
         <v>4</v>
       </c>
-      <c r="G21" s="30"/>
+      <c r="G21" s="36"/>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="10"/>
@@ -1335,9 +1369,9 @@
       <c r="D22" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="36"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="30"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="36"/>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="10">
@@ -1352,11 +1386,11 @@
       <c r="D23" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="E23" s="36"/>
+      <c r="E23" s="31"/>
       <c r="F23" s="22">
         <v>5</v>
       </c>
-      <c r="G23" s="30"/>
+      <c r="G23" s="36"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="10">
@@ -1371,11 +1405,11 @@
       <c r="D24" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E24" s="36"/>
-      <c r="F24" s="32">
+      <c r="E24" s="31"/>
+      <c r="F24" s="34">
         <v>3</v>
       </c>
-      <c r="G24" s="30"/>
+      <c r="G24" s="36"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="10"/>
@@ -1386,9 +1420,9 @@
       <c r="D25" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E25" s="36"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="30"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="36"/>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="10">
@@ -1403,11 +1437,11 @@
       <c r="D26" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E26" s="36"/>
-      <c r="F26" s="32">
+      <c r="E26" s="31"/>
+      <c r="F26" s="34">
         <v>5</v>
       </c>
-      <c r="G26" s="30"/>
+      <c r="G26" s="36"/>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="10"/>
@@ -1418,15 +1452,15 @@
       <c r="D27" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E27" s="36"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="30"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="36"/>
     </row>
     <row r="28" spans="1:7" ht="15" thickBot="1">
       <c r="A28" s="14">
         <v>13</v>
       </c>
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="27" t="s">
         <v>84</v>
       </c>
       <c r="C28" s="16">
@@ -1435,11 +1469,11 @@
       <c r="D28" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="36"/>
+      <c r="E28" s="31"/>
       <c r="F28" s="22">
         <v>4</v>
       </c>
-      <c r="G28" s="30"/>
+      <c r="G28" s="36"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="7">
@@ -1454,11 +1488,13 @@
       <c r="D29" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="E29" s="37"/>
-      <c r="F29" s="32">
+      <c r="E29" s="32"/>
+      <c r="F29" s="34">
         <v>3</v>
       </c>
-      <c r="G29" s="31"/>
+      <c r="G29" s="35">
+        <v>3</v>
+      </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="10"/>
@@ -1469,9 +1505,9 @@
       <c r="D30" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E30" s="38"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="30"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="36"/>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="10">
@@ -1486,11 +1522,11 @@
       <c r="D31" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="E31" s="38"/>
+      <c r="E31" s="33"/>
       <c r="F31" s="22">
         <v>2</v>
       </c>
-      <c r="G31" s="30"/>
+      <c r="G31" s="36"/>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="10">
@@ -1505,11 +1541,11 @@
       <c r="D32" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E32" s="38"/>
+      <c r="E32" s="33"/>
       <c r="F32" s="22">
         <v>2</v>
       </c>
-      <c r="G32" s="30"/>
+      <c r="G32" s="36"/>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="10">
@@ -1520,11 +1556,11 @@
       </c>
       <c r="C33" s="12"/>
       <c r="D33" s="13"/>
-      <c r="E33" s="38"/>
+      <c r="E33" s="33"/>
       <c r="F33" s="22">
         <v>1</v>
       </c>
-      <c r="G33" s="30"/>
+      <c r="G33" s="36"/>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="10">
@@ -1535,11 +1571,11 @@
       </c>
       <c r="C34" s="12"/>
       <c r="D34" s="13"/>
-      <c r="E34" s="38"/>
+      <c r="E34" s="33"/>
       <c r="F34" s="22">
         <v>2</v>
       </c>
-      <c r="G34" s="30"/>
+      <c r="G34" s="36"/>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="14">
@@ -1549,12 +1585,12 @@
         <v>52</v>
       </c>
       <c r="C35" s="16"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="38"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="33"/>
       <c r="F35" s="22">
         <v>12</v>
       </c>
-      <c r="G35" s="30"/>
+      <c r="G35" s="36"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="7">
@@ -1565,11 +1601,13 @@
       </c>
       <c r="C36" s="9"/>
       <c r="D36" s="18"/>
-      <c r="E36" s="35"/>
+      <c r="E36" s="30"/>
       <c r="F36" s="22">
         <v>1.5</v>
       </c>
-      <c r="G36" s="31"/>
+      <c r="G36" s="35">
+        <v>4</v>
+      </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="10">
@@ -1582,11 +1620,11 @@
       <c r="D37" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E37" s="36"/>
+      <c r="E37" s="31"/>
       <c r="F37" s="22">
         <v>2</v>
       </c>
-      <c r="G37" s="30"/>
+      <c r="G37" s="36"/>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="10">
@@ -1597,11 +1635,11 @@
       </c>
       <c r="C38" s="12"/>
       <c r="D38" s="13"/>
-      <c r="E38" s="36"/>
+      <c r="E38" s="31"/>
       <c r="F38" s="22">
         <v>2.5</v>
       </c>
-      <c r="G38" s="30"/>
+      <c r="G38" s="36"/>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="10">
@@ -1614,11 +1652,11 @@
       <c r="D39" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="E39" s="36"/>
+      <c r="E39" s="31"/>
       <c r="F39" s="22">
         <v>7</v>
       </c>
-      <c r="G39" s="30"/>
+      <c r="G39" s="36"/>
     </row>
     <row r="40" spans="1:7" ht="15" thickBot="1">
       <c r="A40" s="14">
@@ -1629,11 +1667,11 @@
       </c>
       <c r="C40" s="16"/>
       <c r="D40" s="21"/>
-      <c r="E40" s="36"/>
+      <c r="E40" s="31"/>
       <c r="F40" s="22">
         <v>3</v>
       </c>
-      <c r="G40" s="30"/>
+      <c r="G40" s="36"/>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="17">
@@ -1648,11 +1686,13 @@
       <c r="D41" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="E41" s="35"/>
-      <c r="F41" s="32">
+      <c r="E41" s="30"/>
+      <c r="F41" s="34">
         <v>7</v>
       </c>
-      <c r="G41" s="31"/>
+      <c r="G41" s="35">
+        <v>5</v>
+      </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="19"/>
@@ -1663,9 +1703,9 @@
       <c r="D42" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="E42" s="36"/>
-      <c r="F42" s="32"/>
-      <c r="G42" s="31"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="34"/>
+      <c r="G42" s="35"/>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="19"/>
@@ -1676,9 +1716,9 @@
       <c r="D43" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="E43" s="36"/>
-      <c r="F43" s="32"/>
-      <c r="G43" s="31"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="34"/>
+      <c r="G43" s="35"/>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="19">
@@ -1693,9 +1733,11 @@
       <c r="D44" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="E44" s="36"/>
-      <c r="F44" s="32"/>
-      <c r="G44" s="31"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="34">
+        <v>10</v>
+      </c>
+      <c r="G44" s="35"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="19"/>
@@ -1706,9 +1748,9 @@
       <c r="D45" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="E45" s="36"/>
-      <c r="F45" s="32"/>
-      <c r="G45" s="31"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="34"/>
+      <c r="G45" s="35"/>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="19"/>
@@ -1719,9 +1761,9 @@
       <c r="D46" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="E46" s="36"/>
-      <c r="F46" s="32"/>
-      <c r="G46" s="31"/>
+      <c r="E46" s="31"/>
+      <c r="F46" s="34"/>
+      <c r="G46" s="35"/>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="19"/>
@@ -1732,9 +1774,9 @@
       <c r="D47" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="E47" s="36"/>
-      <c r="F47" s="32"/>
-      <c r="G47" s="31"/>
+      <c r="E47" s="31"/>
+      <c r="F47" s="34"/>
+      <c r="G47" s="35"/>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="19"/>
@@ -1745,9 +1787,9 @@
       <c r="D48" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="E48" s="36"/>
-      <c r="F48" s="32"/>
-      <c r="G48" s="31"/>
+      <c r="E48" s="31"/>
+      <c r="F48" s="34"/>
+      <c r="G48" s="35"/>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="19"/>
@@ -1758,9 +1800,9 @@
       <c r="D49" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="E49" s="36"/>
-      <c r="F49" s="32"/>
-      <c r="G49" s="31"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="34"/>
+      <c r="G49" s="35"/>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="20"/>
@@ -1771,9 +1813,9 @@
       <c r="D50" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="E50" s="36"/>
-      <c r="F50" s="32"/>
-      <c r="G50" s="31"/>
+      <c r="E50" s="31"/>
+      <c r="F50" s="34"/>
+      <c r="G50" s="35"/>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="17">
@@ -1788,9 +1830,13 @@
       <c r="D51" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="E51" s="33"/>
-      <c r="F51" s="32"/>
-      <c r="G51" s="31"/>
+      <c r="E51" s="28"/>
+      <c r="F51" s="34">
+        <v>8</v>
+      </c>
+      <c r="G51" s="35">
+        <v>6</v>
+      </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="19"/>
@@ -1801,11 +1847,11 @@
       <c r="D52" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="E52" s="34"/>
-      <c r="F52" s="32"/>
-      <c r="G52" s="30"/>
-    </row>
-    <row r="53" spans="1:7">
+      <c r="E52" s="29"/>
+      <c r="F52" s="34"/>
+      <c r="G52" s="36"/>
+    </row>
+    <row r="53" spans="1:7" ht="15" thickBot="1">
       <c r="A53" s="20"/>
       <c r="B53" s="15"/>
       <c r="C53" s="16">
@@ -1814,9 +1860,9 @@
       <c r="D53" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="E53" s="34"/>
-      <c r="F53" s="32"/>
-      <c r="G53" s="30"/>
+      <c r="E53" s="29"/>
+      <c r="F53" s="34"/>
+      <c r="G53" s="36"/>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="17">
@@ -1831,8 +1877,11 @@
       <c r="D54" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="E54" s="34"/>
-      <c r="F54" s="23"/>
+      <c r="E54" s="29"/>
+      <c r="F54" s="38"/>
+      <c r="G54" s="36">
+        <v>7</v>
+      </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="19"/>
@@ -1843,10 +1892,11 @@
       <c r="D55" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="E55" s="34"/>
-      <c r="F55" s="23"/>
-    </row>
-    <row r="56" spans="1:7">
+      <c r="E55" s="29"/>
+      <c r="F55" s="39"/>
+      <c r="G55" s="36"/>
+    </row>
+    <row r="56" spans="1:7" ht="15" thickBot="1">
       <c r="A56" s="20"/>
       <c r="B56" s="15"/>
       <c r="C56" s="16">
@@ -1855,8 +1905,9 @@
       <c r="D56" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="E56" s="34"/>
-      <c r="F56" s="23"/>
+      <c r="E56" s="29"/>
+      <c r="F56" s="40"/>
+      <c r="G56" s="36"/>
     </row>
     <row r="57" spans="1:7">
       <c r="D57" s="3"/>
@@ -1871,22 +1922,9 @@
       <c r="E59" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="E51:E53"/>
-    <mergeCell ref="E54:E56"/>
-    <mergeCell ref="E2:E19"/>
-    <mergeCell ref="E20:E28"/>
-    <mergeCell ref="E29:E35"/>
-    <mergeCell ref="E36:E40"/>
-    <mergeCell ref="E41:E50"/>
-    <mergeCell ref="F51:F53"/>
-    <mergeCell ref="G51:G53"/>
-    <mergeCell ref="G20:G28"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G35"/>
+  <mergeCells count="28">
+    <mergeCell ref="G54:G56"/>
+    <mergeCell ref="F54:F56"/>
     <mergeCell ref="G2:G19"/>
     <mergeCell ref="G36:G40"/>
     <mergeCell ref="F41:F43"/>
@@ -1898,6 +1936,21 @@
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="F13:F15"/>
     <mergeCell ref="F16:F18"/>
+    <mergeCell ref="F51:F53"/>
+    <mergeCell ref="G51:G53"/>
+    <mergeCell ref="G20:G28"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G35"/>
+    <mergeCell ref="E51:E53"/>
+    <mergeCell ref="E54:E56"/>
+    <mergeCell ref="E2:E19"/>
+    <mergeCell ref="E20:E28"/>
+    <mergeCell ref="E29:E35"/>
+    <mergeCell ref="E36:E40"/>
+    <mergeCell ref="E41:E50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>